<commit_message>
agregue descripcion escrita del modelo de negocio y una peque correcion al caso de uso
</commit_message>
<xml_diff>
--- a/Modelo de Requerimiento -Tabla de caso de uso.xlsx
+++ b/Modelo de Requerimiento -Tabla de caso de uso.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ingenieria de software\proyectoDeliberyApp.git\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8250"/>
   </bookViews>
@@ -75,9 +80,6 @@
     <t>6- El recepcionista anota al cliente , en el cuaderno de clientes</t>
   </si>
   <si>
-    <t xml:space="preserve">7- El recepcionista registra el pedido, en el cuadeno de pedidos </t>
-  </si>
-  <si>
     <t>8- El recepcionista elabora el comprobante</t>
   </si>
   <si>
@@ -88,6 +90,9 @@
   </si>
   <si>
     <t>10- El repartidor entrega el pedido y el comprobante al cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7- El recepcionista registra el pedido, en el cuaderno de pedidos </t>
   </si>
 </sst>
 </file>
@@ -321,19 +326,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -346,10 +345,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -361,6 +366,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -409,7 +417,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -444,7 +452,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -656,7 +664,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A20" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,99 +718,99 @@
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="12"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="13"/>
+      <c r="B7" s="26"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="24"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="24"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="24"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="18"/>
+      <c r="B11" s="24"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="18"/>
+      <c r="B12" s="24"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="18"/>
+      <c r="B13" s="24"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="24"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="18"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="B15" s="24"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="18"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="B16" s="24"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="24"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="18"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="18"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="26"/>
+      <c r="B18" s="16"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="24"/>
+      <c r="B19" s="22"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="14" t="s">
         <v>11</v>
       </c>
     </row>
@@ -862,6 +870,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -872,11 +885,6 @@
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificaciones al caso de uso de Modelo de Requerimiento
</commit_message>
<xml_diff>
--- a/Modelo de Requerimiento -Tabla de caso de uso.xlsx
+++ b/Modelo de Requerimiento -Tabla de caso de uso.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ingenieria de software\proyectoDeliberyApp.git\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="8250"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Nombre:</t>
   </si>
@@ -44,9 +39,6 @@
     <t>Autores:</t>
   </si>
   <si>
-    <t>Cliente,Recepcionista,repartidor</t>
-  </si>
-  <si>
     <t>Precondiciones:</t>
   </si>
   <si>
@@ -65,34 +57,43 @@
     <t xml:space="preserve">1 - El Cliente llama por telefono al restaurante </t>
   </si>
   <si>
-    <t>2- La recepcionista contesta la llamada</t>
-  </si>
-  <si>
-    <t>3- El cliente consulta las opciones de  comidas</t>
-  </si>
-  <si>
-    <t>4- El cliente elige y solicita las opciones de comida</t>
-  </si>
-  <si>
-    <t>5- El recepcionista revisa la lista de comidas del restaurant</t>
-  </si>
-  <si>
-    <t>6- El recepcionista anota al cliente , en el cuaderno de clientes</t>
-  </si>
-  <si>
-    <t>8- El recepcionista elabora el comprobante</t>
-  </si>
-  <si>
-    <t>9- El recepcionista entrega el comprobante  al repatidor</t>
-  </si>
-  <si>
-    <t>11 - El cliente recibe el comprobante y el pedido, y paga este</t>
-  </si>
-  <si>
-    <t>10- El repartidor entrega el pedido y el comprobante al cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7- El recepcionista registra el pedido, en el cuaderno de pedidos </t>
+    <t xml:space="preserve">4- La recepcionista le dicta el menu </t>
+  </si>
+  <si>
+    <t>9- La  recepcionista solicita los datos personales al cliente(nombre,apellido,direccion,numero telefono)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5- El cliente elige el menu   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6- La recepcionista anota al cliente su pedido </t>
+  </si>
+  <si>
+    <t>10- La recepcionista comunica el tiempo estimado en que llegara el pedido  finaliza la llamada</t>
+  </si>
+  <si>
+    <t>3- El cliente consulta las opciones de  comidas.( en caso de que el cliente ya sabe lo que quiere pasamos al paso 5)</t>
+  </si>
+  <si>
+    <t>7 -La recepcionista Pregunta si quiere agregar algo mas  a su pedido</t>
+  </si>
+  <si>
+    <t>11-El cliente le da su Ok y finaliza la llamada</t>
+  </si>
+  <si>
+    <t>12-La recepcionista pasa el pedido a la cocina</t>
+  </si>
+  <si>
+    <t>*El cliente debe de dar sus datos personales solicitados</t>
+  </si>
+  <si>
+    <t>8- En caso d que el cliente ya  este sastifecho con su pedido solo confirma  o si desea algo mas volvemos al paso 5</t>
+  </si>
+  <si>
+    <t>2- La recepcionista contesta la llamada y pregunta que se le oferce</t>
+  </si>
+  <si>
+    <t>Cliente,Recepcionista</t>
   </si>
 </sst>
 </file>
@@ -124,7 +125,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -293,11 +294,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -326,37 +378,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,7 +478,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -452,7 +513,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -661,16 +722,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B20"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="63.140625" customWidth="1"/>
+    <col min="2" max="2" width="93.42578125" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -703,7 +764,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -711,129 +772,144 @@
         <v>6</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="23" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="26"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="24"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="B11" s="22"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="24"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="24"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="24"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="B16" s="27"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="24"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="24"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="24"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="24"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="B17" s="27"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="24"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="24"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="B18" s="27"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="16"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="B19" s="29"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
+      <c r="B20" s="31"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="25"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="21"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="22"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="4"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
@@ -865,26 +941,25 @@
     <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C43" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>